<commit_message>
getting a toy ar1 to basic visuals
</commit_message>
<xml_diff>
--- a/stipm_pops_crosscheck.xlsx
+++ b/stipm_pops_crosscheck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/ST-IPM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_501C1CC78F79A8D366075C52F37BD2724A4446D1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D029511E-B3D8-4C1A-9881-E258D6EB39FE}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="11_501C1CC78F79A8D366075C52F37BD2724A4446D1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CD520484-5296-49D6-9723-56C6F3982FAC}"/>
   <bookViews>
-    <workbookView xWindow="-16340" yWindow="-21410" windowWidth="20220" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6090" yWindow="-20330" windowWidth="20220" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,12 +352,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -372,11 +402,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,7 +753,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1117,44 +1152,44 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
-        <v>1986</v>
-      </c>
-      <c r="D11">
-        <v>2017</v>
-      </c>
-      <c r="E11">
-        <v>32</v>
-      </c>
-      <c r="F11">
+      <c r="C11" s="3">
+        <v>1986</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2017</v>
+      </c>
+      <c r="E11" s="3">
+        <v>32</v>
+      </c>
+      <c r="F11" s="3">
         <v>31</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>31</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
         <v>13</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="3" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1196,44 +1231,44 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13">
-        <v>1986</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="6">
+        <v>1986</v>
+      </c>
+      <c r="D13" s="6">
         <v>2018</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>33</v>
       </c>
-      <c r="F13">
-        <v>32</v>
-      </c>
-      <c r="G13">
-        <v>32</v>
-      </c>
-      <c r="H13">
-        <v>32</v>
-      </c>
-      <c r="I13">
+      <c r="F13" s="6">
+        <v>32</v>
+      </c>
+      <c r="G13" s="6">
+        <v>32</v>
+      </c>
+      <c r="H13" s="6">
+        <v>32</v>
+      </c>
+      <c r="I13" s="6">
         <v>30</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="6">
         <v>149</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="6" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1275,44 +1310,44 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15">
-        <v>1986</v>
-      </c>
-      <c r="D15">
-        <v>2017</v>
-      </c>
-      <c r="E15">
-        <v>32</v>
-      </c>
-      <c r="F15">
-        <v>32</v>
-      </c>
-      <c r="G15">
-        <v>32</v>
-      </c>
-      <c r="H15">
+      <c r="C15" s="4">
+        <v>1986</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2017</v>
+      </c>
+      <c r="E15" s="4">
+        <v>32</v>
+      </c>
+      <c r="F15" s="4">
+        <v>32</v>
+      </c>
+      <c r="G15" s="4">
+        <v>32</v>
+      </c>
+      <c r="H15" s="2">
         <v>13</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="4">
         <v>10</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="4">
         <v>107</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1354,126 +1389,126 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
-        <v>1986</v>
-      </c>
-      <c r="D17">
-        <v>2017</v>
-      </c>
-      <c r="E17">
-        <v>32</v>
-      </c>
-      <c r="F17">
-        <v>32</v>
-      </c>
-      <c r="G17">
-        <v>32</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
+      <c r="C17" s="5">
+        <v>1986</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2017</v>
+      </c>
+      <c r="E17" s="5">
+        <v>32</v>
+      </c>
+      <c r="F17" s="5">
+        <v>32</v>
+      </c>
+      <c r="G17" s="5">
+        <v>32</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
         <v>111</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18">
-        <v>1986</v>
-      </c>
-      <c r="D18">
-        <v>2017</v>
-      </c>
-      <c r="E18">
-        <v>32</v>
-      </c>
-      <c r="F18">
+      <c r="C18" s="6">
+        <v>1986</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2017</v>
+      </c>
+      <c r="E18" s="6">
+        <v>32</v>
+      </c>
+      <c r="F18" s="6">
         <v>30</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <v>30</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
+      <c r="J18" s="6">
         <v>157</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19">
-        <v>1986</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="4">
+        <v>1986</v>
+      </c>
+      <c r="D19" s="4">
         <v>2018</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>33</v>
       </c>
-      <c r="F19">
-        <v>32</v>
-      </c>
-      <c r="G19">
-        <v>32</v>
-      </c>
-      <c r="H19">
+      <c r="F19" s="4">
+        <v>32</v>
+      </c>
+      <c r="G19" s="4">
+        <v>32</v>
+      </c>
+      <c r="H19" s="2">
         <v>19</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="4">
         <v>28</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <v>97</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1515,82 +1550,82 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C21">
-        <v>1986</v>
-      </c>
-      <c r="D21">
-        <v>2017</v>
-      </c>
-      <c r="E21">
-        <v>32</v>
-      </c>
-      <c r="F21">
-        <v>32</v>
-      </c>
-      <c r="G21">
-        <v>32</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
+      <c r="C21" s="6">
+        <v>1986</v>
+      </c>
+      <c r="D21" s="6">
+        <v>2017</v>
+      </c>
+      <c r="E21" s="6">
+        <v>32</v>
+      </c>
+      <c r="F21" s="6">
+        <v>32</v>
+      </c>
+      <c r="G21" s="6">
+        <v>32</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
         <v>153</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C22">
-        <v>1986</v>
-      </c>
-      <c r="D22">
-        <v>2017</v>
-      </c>
-      <c r="E22">
-        <v>32</v>
-      </c>
-      <c r="F22">
-        <v>32</v>
-      </c>
-      <c r="G22">
-        <v>32</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
+      <c r="C22" s="4">
+        <v>1986</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2017</v>
+      </c>
+      <c r="E22" s="4">
+        <v>32</v>
+      </c>
+      <c r="F22" s="4">
+        <v>32</v>
+      </c>
+      <c r="G22" s="4">
+        <v>32</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
         <v>101</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1632,85 +1667,85 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C24">
-        <v>1986</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="5">
+        <v>1986</v>
+      </c>
+      <c r="D24" s="5">
         <v>2018</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>33</v>
       </c>
-      <c r="F24">
-        <v>32</v>
-      </c>
-      <c r="G24">
-        <v>32</v>
-      </c>
-      <c r="H24">
+      <c r="F24" s="5">
+        <v>32</v>
+      </c>
+      <c r="G24" s="5">
+        <v>32</v>
+      </c>
+      <c r="H24" s="2">
         <v>14</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="5">
         <v>29</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="5">
         <v>1</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25">
-        <v>1986</v>
-      </c>
-      <c r="D25">
-        <v>2017</v>
-      </c>
-      <c r="E25">
+      <c r="B25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1986</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2017</v>
+      </c>
+      <c r="E25" s="3">
         <v>26</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>25</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>25</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
         <v>43</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1752,41 +1787,41 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C27">
-        <v>1986</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="6">
+        <v>1986</v>
+      </c>
+      <c r="D27" s="6">
         <v>2018</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="6">
         <v>33</v>
       </c>
-      <c r="F27">
-        <v>32</v>
-      </c>
-      <c r="G27">
-        <v>32</v>
-      </c>
-      <c r="H27">
+      <c r="F27" s="6">
+        <v>32</v>
+      </c>
+      <c r="G27" s="6">
+        <v>32</v>
+      </c>
+      <c r="H27" s="6">
         <v>33</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
+      <c r="I27" s="6">
+        <v>0</v>
+      </c>
+      <c r="J27" s="6">
         <v>139</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="6" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1866,44 +1901,44 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="30" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C30">
-        <v>1986</v>
-      </c>
-      <c r="D30">
-        <v>2017</v>
-      </c>
-      <c r="E30">
-        <v>32</v>
-      </c>
-      <c r="F30">
-        <v>32</v>
-      </c>
-      <c r="G30">
-        <v>32</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
+      <c r="C30" s="6">
+        <v>1986</v>
+      </c>
+      <c r="D30" s="6">
+        <v>2017</v>
+      </c>
+      <c r="E30" s="6">
+        <v>32</v>
+      </c>
+      <c r="F30" s="6">
+        <v>32</v>
+      </c>
+      <c r="G30" s="6">
+        <v>32</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0</v>
+      </c>
+      <c r="I30" s="6">
         <v>29</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="6">
         <v>145</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="6" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>